<commit_message>
updated tool and docs;
</commit_message>
<xml_diff>
--- a/Budgeting-and-Financial-Planning-Tools.xlsx
+++ b/Budgeting-and-Financial-Planning-Tools.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="203">
   <si>
     <t>Car Insurance</t>
   </si>
@@ -149,12 +149,6 @@
     <t>Risk</t>
   </si>
   <si>
-    <t>Limit</t>
-  </si>
-  <si>
-    <t>Cashflow</t>
-  </si>
-  <si>
     <t>DirectTV</t>
   </si>
   <si>
@@ -299,9 +293,6 @@
     <t>Maybe substitute netflix + 5 CBS All Access kind of things if it keeps going up</t>
   </si>
   <si>
-    <t>Debt to Cashflow</t>
-  </si>
-  <si>
     <t>Paid</t>
   </si>
   <si>
@@ -584,9 +575,6 @@
     <t>Tina Mom Student Loans</t>
   </si>
   <si>
-    <t>Rate per D2C</t>
-  </si>
-  <si>
     <t>Investing is a different animal than paying off bills; don't directly compare this line to bills</t>
   </si>
   <si>
@@ -608,6 +596,9 @@
     <t>EOM info = BOM for next period to create a "chain."</t>
   </si>
   <si>
+    <t>Time to Parity</t>
+  </si>
+  <si>
     <t>Weighted Time to Parity</t>
   </si>
   <si>
@@ -617,7 +608,28 @@
     <t>Weighted Time Debt</t>
   </si>
   <si>
-    <t>Time to Parity (Principle/Interest-Ignorant)</t>
+    <t>Cash Flow-to-Debt</t>
+  </si>
+  <si>
+    <t>Janky Debt</t>
+  </si>
+  <si>
+    <t>Fictional</t>
+  </si>
+  <si>
+    <t>Choose Lowest - Principle/Interest-Ignorant</t>
+  </si>
+  <si>
+    <t>Janky Parity</t>
+  </si>
+  <si>
+    <t>Account Value (Absolute Value)</t>
+  </si>
+  <si>
+    <t>Cash Flow / Monthly Account Expenditure</t>
+  </si>
+  <si>
+    <t>Use the monthly amount paid in to a preferred stock account, not the dividend income.</t>
   </si>
 </sst>
 </file>
@@ -1089,7 +1101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V75"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -1109,10 +1121,10 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>17</v>
@@ -1121,19 +1133,19 @@
         <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>18</v>
@@ -1142,7 +1154,7 @@
     <row r="2" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>19</v>
@@ -1159,19 +1171,19 @@
         <v>-55</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>120</v>
-      </c>
       <c r="K2" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>20</v>
@@ -1188,13 +1200,13 @@
         <v>-266.66666666666674</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>21</v>
@@ -1211,13 +1223,13 @@
         <v>-133.33333333333337</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>22</v>
@@ -1234,13 +1246,13 @@
         <v>-33.333333333333343</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>23</v>
@@ -1257,13 +1269,13 @@
         <v>-33.333333333333343</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -1280,12 +1292,12 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I7"/>
       <c r="J7" s="26"/>
       <c r="K7" s="26" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L7" s="26"/>
       <c r="M7" s="26"/>
@@ -1301,10 +1313,10 @@
     <row r="8" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D8">
         <v>-240</v>
@@ -1319,7 +1331,7 @@
         <v>-80</v>
       </c>
       <c r="H8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I8"/>
       <c r="J8"/>
@@ -1338,10 +1350,10 @@
     <row r="9" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D9">
         <v>-125</v>
@@ -1356,11 +1368,11 @@
         <v>-41.666666666666671</v>
       </c>
       <c r="H9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I9"/>
       <c r="J9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K9"/>
       <c r="L9"/>
@@ -1378,10 +1390,10 @@
     <row r="10" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D10">
         <v>-80</v>
@@ -1396,7 +1408,7 @@
         <v>-26.666666666666671</v>
       </c>
       <c r="H10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -1418,7 +1430,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>
@@ -1435,14 +1447,14 @@
         <v>0</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I11">
         <v>365000</v>
       </c>
       <c r="J11" s="26"/>
       <c r="K11" s="26" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="L11" s="26"/>
       <c r="M11" s="26"/>
@@ -1461,7 +1473,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -1478,7 +1490,7 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I12"/>
       <c r="J12" s="26"/>
@@ -1500,7 +1512,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -1516,7 +1528,7 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J13" s="26"/>
       <c r="K13" s="26"/>
@@ -1535,10 +1547,10 @@
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D14" s="5">
         <v>-25</v>
@@ -1552,7 +1564,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -1574,7 +1586,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>1</v>
@@ -1591,7 +1603,7 @@
         <v>39</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I15" s="4">
         <v>1800</v>
@@ -1615,7 +1627,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
@@ -1632,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="26"/>
@@ -1654,10 +1666,10 @@
         <v>9</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D17" s="4">
         <v>-70</v>
@@ -1671,7 +1683,7 @@
         <v>30</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I17" s="4">
         <v>3800</v>
@@ -1695,7 +1707,7 @@
         <v>13</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
@@ -1711,7 +1723,7 @@
         <v>-46</v>
       </c>
       <c r="H18" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J18" s="26"/>
       <c r="K18" s="26"/>
@@ -1732,10 +1744,10 @@
         <v>13</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D19">
         <v>-60</v>
@@ -1748,7 +1760,7 @@
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="V19" s="26"/>
     </row>
@@ -1757,10 +1769,10 @@
         <v>42385</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D20">
         <v>-192</v>
@@ -1779,10 +1791,10 @@
         <v>42389</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D21">
         <v>-30</v>
@@ -1795,7 +1807,7 @@
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="V21" s="26"/>
     </row>
@@ -1804,10 +1816,10 @@
         <v>10</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D22">
         <v>-30</v>
@@ -1820,7 +1832,7 @@
         <v>135</v>
       </c>
       <c r="H22" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I22">
         <v>1720</v>
@@ -1832,7 +1844,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>7</v>
@@ -1849,7 +1861,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="29" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
@@ -1870,10 +1882,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D24" s="4">
         <v>-25</v>
@@ -1887,7 +1899,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I24" s="4">
         <v>1450</v>
@@ -1910,7 +1922,7 @@
         <v>15</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
@@ -1926,12 +1938,12 @@
         <v>0</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="26"/>
       <c r="K25" s="26" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="L25" s="26"/>
       <c r="M25" s="26"/>
@@ -1949,10 +1961,10 @@
         <v>42390</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C26" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D26">
         <v>-75</v>
@@ -1965,10 +1977,10 @@
         <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K26" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
@@ -1976,10 +1988,10 @@
         <v>42390</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C27" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D27">
         <v>-150</v>
@@ -1990,13 +2002,13 @@
         <v>-150</v>
       </c>
       <c r="H27" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I27">
         <v>-1285</v>
       </c>
       <c r="K27" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
@@ -2004,7 +2016,7 @@
         <v>31</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
@@ -2018,7 +2030,7 @@
         <v>-40</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="26"/>
@@ -2039,7 +2051,7 @@
         <v>42393</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
@@ -2055,7 +2067,7 @@
         <v>0</v>
       </c>
       <c r="H29" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I29">
         <v>10890</v>
@@ -2078,7 +2090,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C30" t="s">
         <v>5</v>
@@ -2092,7 +2104,7 @@
         <v>-75</v>
       </c>
       <c r="H30" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
@@ -2100,10 +2112,10 @@
         <v>31</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D31">
         <v>-70</v>
@@ -2113,10 +2125,10 @@
         <v>-70</v>
       </c>
       <c r="H31" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
@@ -2124,10 +2136,10 @@
         <v>42391</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D32">
         <v>-30</v>
@@ -2137,10 +2149,10 @@
         <v>-30</v>
       </c>
       <c r="H32" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K32" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2148,23 +2160,23 @@
         <v>42391</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C33" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G33" s="3"/>
       <c r="K33" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C34" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D34">
         <v>-75</v>
@@ -2174,10 +2186,10 @@
         <v>-75</v>
       </c>
       <c r="H34" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="K34" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2185,10 +2197,10 @@
         <v>5</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -2201,10 +2213,10 @@
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -2217,7 +2229,7 @@
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C37" t="s">
         <v>14</v>
@@ -2236,7 +2248,7 @@
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
       <c r="B38" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C38" t="s">
         <v>15</v>
@@ -2255,7 +2267,7 @@
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
         <v>14</v>
@@ -2271,7 +2283,7 @@
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="B40" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C40" t="s">
         <v>15</v>
@@ -2287,7 +2299,7 @@
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
       <c r="B41" s="12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C41" t="s">
         <v>14</v>
@@ -2303,7 +2315,7 @@
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C42" t="s">
         <v>15</v>
@@ -2318,10 +2330,10 @@
     </row>
     <row r="43" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D43" s="16" t="e">
         <f>SUM(D2:D10)/4+#REF!/4+D34/4</f>
@@ -2343,7 +2355,7 @@
     <row r="44" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22"/>
       <c r="B44" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D44" s="16" t="e">
         <f>SUM(D11:D13)+D43</f>
@@ -2367,7 +2379,7 @@
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
       <c r="B45" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D45" s="16" t="e">
         <f>SUM(D14:D22)+D43</f>
@@ -2388,7 +2400,7 @@
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="22"/>
       <c r="B46" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D46" s="16" t="e">
         <f>SUM(D23:D27)+D43</f>
@@ -2410,7 +2422,7 @@
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="23"/>
       <c r="B47" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D47" s="16" t="e">
         <f>SUM(D28:D33)+D43</f>
@@ -2432,7 +2444,7 @@
     <row r="48" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="21"/>
       <c r="B48" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D48" s="8">
         <f>SUM(D2:D42)</f>
@@ -2457,7 +2469,7 @@
     </row>
     <row r="49" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G49" s="2">
         <f>G48-F48</f>
@@ -2469,12 +2481,12 @@
     </row>
     <row r="51" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="52" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C52" s="2" t="str">
         <f>IF(D52=E52,"PASS","FAIL")</f>
@@ -2491,7 +2503,7 @@
     </row>
     <row r="53" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C53" s="2" t="e">
         <f>IF(AND(D53=E53,E53=F53),"PASS","FAIL")</f>
@@ -2513,12 +2525,12 @@
     <row r="54" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="9"/>
       <c r="D54" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E55">
         <v>30</v>
@@ -2526,7 +2538,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E56">
         <v>20</v>
@@ -2534,18 +2546,18 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E58">
         <v>1250</v>
       </c>
       <c r="K58" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E59">
         <v>2540</v>
@@ -2553,7 +2565,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E60">
         <f>E58+G49</f>
@@ -2562,7 +2574,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E61" s="30">
         <f>E59+G49</f>
@@ -2571,7 +2583,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E63">
         <f>C71</f>
@@ -2580,7 +2592,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E64">
         <f>E60-E63</f>
@@ -2589,7 +2601,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E65">
         <f>D71</f>
@@ -2598,7 +2610,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E66" s="30">
         <f>E61-E65</f>
@@ -2607,21 +2619,21 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>142</v>
+      </c>
+      <c r="C68" t="s">
+        <v>143</v>
+      </c>
+      <c r="D68" t="s">
+        <v>144</v>
+      </c>
+      <c r="E68" t="s">
         <v>145</v>
-      </c>
-      <c r="C68" t="s">
-        <v>146</v>
-      </c>
-      <c r="D68" t="s">
-        <v>147</v>
-      </c>
-      <c r="E68" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C69">
         <v>1793</v>
@@ -2632,7 +2644,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -2663,17 +2675,17 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -2700,16 +2712,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2723,7 +2735,7 @@
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2737,7 +2749,7 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2751,7 +2763,7 @@
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2765,7 +2777,7 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2779,7 +2791,7 @@
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2793,7 +2805,7 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2807,7 +2819,7 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2821,7 +2833,7 @@
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2835,7 +2847,7 @@
         <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2849,7 +2861,7 @@
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2863,7 +2875,7 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2877,7 +2889,7 @@
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2891,7 +2903,7 @@
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2905,7 +2917,7 @@
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2919,7 +2931,7 @@
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2933,7 +2945,7 @@
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2947,7 +2959,7 @@
         <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2961,7 +2973,7 @@
         <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2975,7 +2987,7 @@
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2989,7 +3001,7 @@
         <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3003,7 +3015,7 @@
         <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3017,7 +3029,7 @@
         <v>19</v>
       </c>
       <c r="D23" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3031,7 +3043,7 @@
         <v>19</v>
       </c>
       <c r="D24" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3045,7 +3057,7 @@
         <v>19</v>
       </c>
       <c r="D25" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3059,7 +3071,7 @@
         <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3073,7 +3085,7 @@
         <v>19</v>
       </c>
       <c r="D27" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3087,7 +3099,7 @@
         <v>19</v>
       </c>
       <c r="D28" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3101,7 +3113,7 @@
         <v>19</v>
       </c>
       <c r="D29" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3115,7 +3127,7 @@
         <v>19</v>
       </c>
       <c r="D30" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3129,7 +3141,7 @@
         <v>19</v>
       </c>
       <c r="D31" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3143,7 +3155,7 @@
         <v>19</v>
       </c>
       <c r="D32" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3157,7 +3169,7 @@
         <v>19</v>
       </c>
       <c r="D33" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3171,7 +3183,7 @@
         <v>19</v>
       </c>
       <c r="D34" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3185,7 +3197,7 @@
         <v>19</v>
       </c>
       <c r="D35" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3199,7 +3211,7 @@
         <v>19</v>
       </c>
       <c r="D36" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3213,7 +3225,7 @@
         <v>19</v>
       </c>
       <c r="D37" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3227,7 +3239,7 @@
         <v>19</v>
       </c>
       <c r="D38" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3241,7 +3253,7 @@
         <v>19</v>
       </c>
       <c r="D39" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3255,7 +3267,7 @@
         <v>19</v>
       </c>
       <c r="D40" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3269,7 +3281,7 @@
         <v>19</v>
       </c>
       <c r="D41" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3283,7 +3295,7 @@
         <v>19</v>
       </c>
       <c r="D42" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3297,7 +3309,7 @@
         <v>19</v>
       </c>
       <c r="D43" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3311,7 +3323,7 @@
         <v>19</v>
       </c>
       <c r="D44" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3325,7 +3337,7 @@
         <v>19</v>
       </c>
       <c r="D45" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3339,7 +3351,7 @@
         <v>19</v>
       </c>
       <c r="D46" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3353,7 +3365,7 @@
         <v>19</v>
       </c>
       <c r="D47" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3367,7 +3379,7 @@
         <v>19</v>
       </c>
       <c r="D48" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3381,7 +3393,7 @@
         <v>19</v>
       </c>
       <c r="D49" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3395,7 +3407,7 @@
         <v>19</v>
       </c>
       <c r="D50" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3409,7 +3421,7 @@
         <v>19</v>
       </c>
       <c r="D51" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3423,7 +3435,7 @@
         <v>19</v>
       </c>
       <c r="D52" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3437,7 +3449,7 @@
         <v>19</v>
       </c>
       <c r="D53" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3451,7 +3463,7 @@
         <v>19</v>
       </c>
       <c r="D54" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3465,7 +3477,7 @@
         <v>19</v>
       </c>
       <c r="D55" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3479,7 +3491,7 @@
         <v>19</v>
       </c>
       <c r="D56" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3493,7 +3505,7 @@
         <v>19</v>
       </c>
       <c r="D57" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -3507,7 +3519,7 @@
         <v>19</v>
       </c>
       <c r="D58" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -3521,7 +3533,7 @@
         <v>19</v>
       </c>
       <c r="D59" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3535,7 +3547,7 @@
         <v>19</v>
       </c>
       <c r="D60" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3549,7 +3561,7 @@
         <v>19</v>
       </c>
       <c r="D61" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3563,7 +3575,7 @@
         <v>19</v>
       </c>
       <c r="D62" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3577,7 +3589,7 @@
         <v>19</v>
       </c>
       <c r="D63" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3591,7 +3603,7 @@
         <v>19</v>
       </c>
       <c r="D64" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -3615,13 +3627,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3774,7 +3786,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C3">
         <v>1310</v>
@@ -3782,7 +3794,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C4">
         <v>980</v>
@@ -3790,7 +3802,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -3798,7 +3810,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -3849,18 +3861,18 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D12">
         <v>380000</v>
       </c>
       <c r="F12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D13">
         <v>9350</v>
@@ -3868,7 +3880,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D14">
         <v>4150</v>
@@ -3876,21 +3888,21 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F15" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E16">
         <v>151500</v>
       </c>
       <c r="F16" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3911,7 +3923,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E19">
         <v>440</v>
@@ -3919,7 +3931,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E20">
         <v>1900</v>
@@ -3943,7 +3955,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E23">
         <v>2000</v>
@@ -3951,7 +3963,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -3959,7 +3971,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -3997,7 +4009,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E28">
         <f>E27-E26</f>
@@ -4039,22 +4051,22 @@
         <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>18</v>
@@ -4065,7 +4077,7 @@
         <v>42370</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D2">
         <v>875</v>
@@ -4087,7 +4099,7 @@
         <v>8.3536030002678796</v>
       </c>
       <c r="M2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -4095,7 +4107,7 @@
         <v>42401</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D3">
         <v>875</v>
@@ -4118,7 +4130,7 @@
         <v>11.812121212121212</v>
       </c>
       <c r="M3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -4126,7 +4138,7 @@
         <v>42430</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C4">
         <v>-3000</v>
@@ -4150,7 +4162,7 @@
         <v>7.6431372549019612</v>
       </c>
       <c r="M4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -4181,7 +4193,7 @@
         <v>6.9856630824372763</v>
       </c>
       <c r="M5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -4210,7 +4222,7 @@
         <v>6.4966666666666661</v>
       </c>
       <c r="M6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -4218,7 +4230,7 @@
         <v>42522</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D7">
         <v>5500</v>
@@ -4233,7 +4245,7 @@
         <v>42552</v>
       </c>
       <c r="B8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C8">
         <v>-1000</v>
@@ -4251,7 +4263,7 @@
         <v>42583</v>
       </c>
       <c r="B9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C9">
         <v>-250</v>
@@ -4299,7 +4311,7 @@
         <v>42675</v>
       </c>
       <c r="B12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C12">
         <v>-250</v>
@@ -4317,7 +4329,7 @@
         <v>42705</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C13">
         <v>-1000</v>
@@ -4337,10 +4349,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:T44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4349,55 +4361,58 @@
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="82.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="82.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>201</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
         <v>41</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>200</v>
       </c>
       <c r="F1" t="s">
-        <v>92</v>
+        <v>195</v>
       </c>
       <c r="G1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="H1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="I1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="J1" t="s">
+        <v>196</v>
+      </c>
+      <c r="K1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B2">
         <v>260</v>
@@ -4406,7 +4421,7 @@
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E2">
         <v>10890</v>
@@ -4416,21 +4431,25 @@
         <v>2.3875114784205693E-2</v>
       </c>
       <c r="G2">
-        <f>C2/F2</f>
-        <v>3.5601923076923079</v>
-      </c>
-      <c r="H2">
         <f>E2/B2</f>
         <v>41.884615384615387</v>
       </c>
+      <c r="H2">
+        <f>G2*(1/C2)</f>
+        <v>492.76018099547508</v>
+      </c>
       <c r="I2">
-        <f>H2*C2</f>
-        <v>3.5601923076923083</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <f>E2/(B2+1)</f>
+        <v>41.724137931034484</v>
+      </c>
+      <c r="J2">
+        <f>I2*(1/(C2+1))</f>
+        <v>38.455426664547915</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4439,7 +4458,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E3">
         <v>21500</v>
@@ -4449,20 +4468,25 @@
         <v>0</v>
       </c>
       <c r="G3" t="e">
-        <f>C3/F3+1</f>
+        <f t="shared" ref="G3:G13" si="0">E3/B3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H3">
-        <v>0</v>
+      <c r="H3" t="e">
+        <f t="shared" ref="H3:H13" si="1">G3*(1/C3)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I12" si="0">H3*C3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="I3:I13" si="2">E3/(B3+1)</f>
+        <v>21500</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J13" si="3">I3*(1/(C3+1))</f>
+        <v>20472.290992191964</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4471,30 +4495,35 @@
         <v>5.5199999999999999E-2</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E4">
         <v>75000</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F6" si="1">B4/E4</f>
+        <f>B4/E4</f>
         <v>0</v>
       </c>
       <c r="G4" t="e">
-        <f t="shared" ref="G3:G12" si="2">C4/F4</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H4">
-        <v>0</v>
+      <c r="H4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>75000</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>71076.573161485983</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4503,28 +4532,33 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E5">
         <v>55000</v>
       </c>
       <c r="F5">
+        <f>B5/E5</f>
+        <v>0</v>
+      </c>
+      <c r="G5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H5" t="e">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G5" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I5">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>55000</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>51643.19248826291</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -4535,29 +4569,33 @@
         <v>3.7499999999999999E-2</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E6">
         <v>364000</v>
       </c>
       <c r="F6">
+        <f>B6/E6</f>
+        <v>6.5934065934065934E-3</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>151.66666666666666</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="1"/>
-        <v>6.5934065934065934E-3</v>
-      </c>
-      <c r="G6">
+        <v>4044.4444444444443</v>
+      </c>
+      <c r="I6">
         <f t="shared" si="2"/>
-        <v>5.6875</v>
-      </c>
-      <c r="H6">
-        <f>E6/B6</f>
-        <v>151.66666666666666</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>5.6874999999999991</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>151.60349854227405</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>146.12385401664966</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -4568,7 +4606,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E7">
         <v>5700</v>
@@ -4578,21 +4616,25 @@
         <v>3.5087719298245612E-2</v>
       </c>
       <c r="G7">
+        <f t="shared" si="0"/>
+        <v>28.5</v>
+      </c>
+      <c r="H7" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <f>E7/B7</f>
-        <v>28.5</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>28.35820895522388</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>28.35820895522388</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B8">
         <v>30</v>
@@ -4601,7 +4643,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E8">
         <v>1720</v>
@@ -4611,21 +4653,25 @@
         <v>1.7441860465116279E-2</v>
       </c>
       <c r="G8">
+        <f t="shared" si="0"/>
+        <v>57.333333333333336</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>197.70114942528738</v>
+      </c>
+      <c r="I8">
         <f t="shared" si="2"/>
-        <v>16.626666666666665</v>
-      </c>
-      <c r="H8">
-        <f>E8/B8</f>
-        <v>57.333333333333336</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>16.626666666666665</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>55.483870967741936</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>43.01075268817204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B9">
         <v>25</v>
@@ -4634,31 +4680,35 @@
         <v>0.14249999999999999</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E9">
         <v>1450</v>
       </c>
       <c r="F9">
-        <f t="shared" ref="F9:F10" si="3">B9/E9</f>
+        <f>B9/E9</f>
         <v>1.7241379310344827E-2</v>
       </c>
       <c r="G9">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>407.01754385964915</v>
+      </c>
+      <c r="I9">
         <f t="shared" si="2"/>
-        <v>8.2649999999999988</v>
-      </c>
-      <c r="H9">
-        <f t="shared" ref="H9:H12" si="4">E9/B9</f>
-        <v>58</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>8.2649999999999988</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>55.769230769230766</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>48.813331089042244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B10">
         <v>70</v>
@@ -4667,29 +4717,33 @@
         <v>0.14249999999999999</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E10">
         <v>3800</v>
       </c>
       <c r="F10">
+        <f>B10/E10</f>
+        <v>1.8421052631578946E-2</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>54.285714285714285</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>380.95238095238096</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>53.521126760563384</v>
+      </c>
+      <c r="J10">
         <f t="shared" si="3"/>
-        <v>1.8421052631578946E-2</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="2"/>
-        <v>7.7357142857142858</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="4"/>
-        <v>54.285714285714285</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>7.7357142857142849</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>46.845625173359636</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -4700,7 +4754,7 @@
         <v>0.1</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E11" s="4">
         <v>1800</v>
@@ -4710,400 +4764,455 @@
         <v>3.6111111111111108E-2</v>
       </c>
       <c r="G11">
+        <f t="shared" si="0"/>
+        <v>27.692307692307693</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>276.92307692307691</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="2"/>
-        <v>2.7692307692307696</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="4"/>
-        <v>27.692307692307693</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>2.7692307692307696</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>27.272727272727273</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>24.793388429752067</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B12">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="C12" s="15">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="D12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E12" s="4">
-        <v>-1285</v>
+        <v>1285</v>
       </c>
       <c r="F12">
         <f>B12/E12</f>
         <v>0.11673151750972763</v>
       </c>
       <c r="G12">
+        <f t="shared" si="0"/>
+        <v>8.5666666666666664</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>244.76190476190473</v>
+      </c>
+      <c r="I12">
         <f t="shared" si="2"/>
-        <v>0.29983333333333334</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="4"/>
+        <v>8.5099337748344368</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>8.2221582365550123</v>
+      </c>
+      <c r="K12" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>197</v>
+      </c>
+      <c r="B13">
+        <v>150</v>
+      </c>
+      <c r="C13" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="D13" t="s">
+        <v>182</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1285</v>
+      </c>
+      <c r="F13">
+        <f>B13/E13</f>
+        <v>0.11673151750972763</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
         <v>8.5666666666666664</v>
       </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>0.29983333333333334</v>
-      </c>
-      <c r="J12" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E13">
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>171.33333333333331</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>8.5099337748344368</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>8.1046988331756538</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>202</v>
+      </c>
+      <c r="E14">
         <f>SUM(E3:E5)</f>
         <v>151500</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>54</v>
       </c>
-      <c r="D19" t="s">
+      <c r="B21" s="14">
+        <v>4500</v>
+      </c>
+      <c r="C21" s="15">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D21" s="14">
+        <f>C21*B21</f>
+        <v>202.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>55</v>
       </c>
-      <c r="E19" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="14">
-        <v>4500</v>
-      </c>
-      <c r="C20" s="15">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="D20" s="14">
-        <f>C20*B20</f>
-        <v>202.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="14">
+      <c r="B22" s="14">
         <v>2341.14</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C22" s="15">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="D21" s="14">
-        <f t="shared" ref="D21:D28" si="5">C21*B21</f>
+      <c r="D22" s="14">
+        <f t="shared" ref="D22:D29" si="4">C22*B22</f>
         <v>159.19752</v>
       </c>
-      <c r="R21" s="15"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" s="14">
+      <c r="S22" s="15"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="14">
         <v>5500</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C23" s="15">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="D22" s="14">
-        <f t="shared" si="5"/>
+      <c r="D23" s="14">
+        <f t="shared" si="4"/>
         <v>187</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" s="14">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="14">
         <v>2219.64</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C24" s="15">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="D23" s="14">
-        <f t="shared" si="5"/>
+      <c r="D24" s="14">
+        <f t="shared" si="4"/>
         <v>150.93552</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="14">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="14">
         <v>2796.61</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C25" s="15">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="D24" s="14">
-        <f t="shared" si="5"/>
+      <c r="D25" s="14">
+        <f t="shared" si="4"/>
         <v>95.084740000000011</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25" s="14">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="14">
         <v>1055.45</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C26" s="15">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="D25" s="14">
-        <f t="shared" si="5"/>
+      <c r="D26" s="14">
+        <f t="shared" si="4"/>
         <v>71.770600000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="14">
-        <v>20500</v>
-      </c>
-      <c r="C26" s="15">
-        <v>5.4100000000000002E-2</v>
-      </c>
-      <c r="D26" s="14">
-        <f t="shared" si="5"/>
-        <v>1109.05</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B27" s="14">
         <v>20500</v>
       </c>
       <c r="C27" s="15">
+        <v>5.4100000000000002E-2</v>
+      </c>
+      <c r="D27" s="14">
+        <f t="shared" si="4"/>
+        <v>1109.05</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="14">
+        <v>20500</v>
+      </c>
+      <c r="C28" s="15">
         <v>6.2100000000000002E-2</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D28" s="14">
+        <f t="shared" si="4"/>
+        <v>1273.05</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="14">
+        <v>10250</v>
+      </c>
+      <c r="C29" s="15">
+        <v>5.8400000000000001E-2</v>
+      </c>
+      <c r="D29" s="14">
+        <f t="shared" si="4"/>
+        <v>598.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="14">
+        <f>SUM(B21:B29)</f>
+        <v>69662.84</v>
+      </c>
+      <c r="D30" s="14">
+        <f>SUM(D21:D29)</f>
+        <v>3847.1883800000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31">
+        <f>D30/B30</f>
+        <v>5.522583317016648E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="14">
+        <v>5500</v>
+      </c>
+      <c r="B35" s="14">
+        <v>4368.74</v>
+      </c>
+      <c r="C35" s="15">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="D35" s="14">
+        <f>C35*B35</f>
+        <v>148.53716</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" s="14">
+        <v>2000</v>
+      </c>
+      <c r="B36" s="14">
+        <v>1656.03</v>
+      </c>
+      <c r="C36" s="15">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="D36" s="14">
+        <f t="shared" ref="D36:D42" si="5">C36*B36</f>
+        <v>112.61004000000001</v>
+      </c>
+      <c r="T36" s="6"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" s="14">
+        <v>4500</v>
+      </c>
+      <c r="B37" s="14">
+        <v>3536.13</v>
+      </c>
+      <c r="C37" s="15">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="D37" s="14">
         <f t="shared" si="5"/>
-        <v>1273.05</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="14">
-        <v>10250</v>
-      </c>
-      <c r="C28" s="15">
-        <v>5.8400000000000001E-2</v>
-      </c>
-      <c r="D28" s="14">
-        <f t="shared" si="5"/>
-        <v>598.6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" s="14">
-        <f>SUM(B20:B28)</f>
-        <v>69662.84</v>
-      </c>
-      <c r="D29" s="14">
-        <f>SUM(D20:D28)</f>
-        <v>3847.1883800000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30">
-        <f>D29/B29</f>
-        <v>5.522583317016648E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="14">
-        <v>5500</v>
-      </c>
-      <c r="B34" s="14">
-        <v>4368.74</v>
-      </c>
-      <c r="C34" s="15">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="D34" s="14">
-        <f>C34*B34</f>
-        <v>148.53716</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="14">
-        <v>2000</v>
-      </c>
-      <c r="B35" s="14">
-        <v>1656.03</v>
-      </c>
-      <c r="C35" s="15">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="D35" s="14">
-        <f t="shared" ref="D35:D41" si="6">C35*B35</f>
-        <v>112.61004000000001</v>
-      </c>
-      <c r="S35" s="6"/>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="14">
-        <v>4500</v>
-      </c>
-      <c r="B36" s="14">
-        <v>3536.13</v>
-      </c>
-      <c r="C36" s="15">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="D36" s="14">
-        <f t="shared" si="6"/>
         <v>120.22842000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="14">
-        <v>3500</v>
-      </c>
-      <c r="B37" s="14">
-        <v>2737.91</v>
-      </c>
-      <c r="C37" s="15">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="D37" s="14">
-        <f t="shared" si="6"/>
-        <v>123.20594999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
         <v>3500</v>
       </c>
       <c r="B38" s="14">
+        <v>2737.91</v>
+      </c>
+      <c r="C38" s="15">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D38" s="14">
+        <f t="shared" si="5"/>
+        <v>123.20594999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" s="14">
+        <v>3500</v>
+      </c>
+      <c r="B39" s="14">
         <v>2641.58</v>
       </c>
-      <c r="C38" s="15">
+      <c r="C39" s="15">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="D38" s="14">
-        <f t="shared" si="6"/>
+      <c r="D39" s="14">
+        <f t="shared" si="5"/>
         <v>147.92848000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="14">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="14">
         <v>2000</v>
       </c>
-      <c r="B39" s="14">
+      <c r="B40" s="14">
         <v>1851.37</v>
-      </c>
-      <c r="C39" s="15">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="D39" s="14">
-        <f t="shared" si="6"/>
-        <v>125.89315999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="14">
-        <v>1975</v>
-      </c>
-      <c r="B40" s="14">
-        <v>1851.36</v>
       </c>
       <c r="C40" s="15">
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="D40" s="14">
-        <f t="shared" si="6"/>
-        <v>125.89248000000001</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>125.89315999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="14">
-        <v>2000</v>
+        <v>1975</v>
       </c>
       <c r="B41" s="14">
-        <v>1767.41</v>
+        <v>1851.36</v>
       </c>
       <c r="C41" s="15">
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="D41" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
+        <v>125.89248000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="14">
+        <v>2000</v>
+      </c>
+      <c r="B42" s="14">
+        <v>1767.41</v>
+      </c>
+      <c r="C42" s="15">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="D42" s="14">
+        <f t="shared" si="5"/>
         <v>120.18388000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B42" s="14">
-        <f>SUM(B34:B41)</f>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="14">
+        <f>SUM(B35:B42)</f>
         <v>20410.53</v>
       </c>
-      <c r="D42" s="14">
-        <f>SUM(D34:D41)</f>
+      <c r="D43" s="14">
+        <f>SUM(D35:D42)</f>
         <v>1024.47957</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>58</v>
-      </c>
-      <c r="C43">
-        <f>D42/B42</f>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44">
+        <f>D43/B43</f>
         <v>5.019367796916592E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5125,10 +5234,10 @@
         <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D1" t="s">
         <v>18</v>
@@ -5136,7 +5245,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B2">
         <v>1000</v>
@@ -5144,7 +5253,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B3">
         <v>300</v>
@@ -5152,7 +5261,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B4">
         <v>3500</v>
@@ -5163,7 +5272,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B5">
         <v>750</v>
@@ -5194,27 +5303,27 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B2">
         <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -5222,13 +5331,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3">
         <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H3">
         <v>50</v>
@@ -5236,13 +5345,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4">
         <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H4">
         <v>100</v>
@@ -5250,13 +5359,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B5">
         <v>50</v>
       </c>
       <c r="G5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H5">
         <v>-100</v>
@@ -5264,7 +5373,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -5272,18 +5381,18 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B7">
         <v>2500</v>
       </c>
       <c r="G7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B8">
         <v>300</v>

</xml_diff>